<commit_message>
fix: Question Translation support (#3514)
* [WIP] Question Import in models.py

* [FINAL] "models.py" Question Translations Support

* Add Question Description Support

* [WIP 1] convert_library_v2.py

* [WIP 2] convert_library_v2.py

* [FINAL] "convert_library_v2.py" Full Questions/Answers Translation support

* Fix Typo

* Code Linting

* Code Lint 2

* Revert "Code Lint 2"

This reverts commit 16ae9fbd041035bc769fa8991e0f3e57fdafde7d.

* Code Lint 3

* Small Type Fix

* Fix Returned Questions if no questions available

* Avoid deepcopy

* ruff

---------

Co-authored-by: eric-intuitem <71850047+eric-intuitem@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tools/example_questionnaire.xlsx
+++ b/tools/example_questionnaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tarkadia\projects\intuitem\ciso-assistant-community\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5973631A-699D-4DEE-A82E-6A4FBE39B650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680A424F-0281-4BCF-81C7-3AEE7D1D4698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1485" yWindow="-15870" windowWidth="25440" windowHeight="15990" tabRatio="907" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1659,7 +1659,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="416">
   <si>
     <t>type</t>
   </si>
@@ -3251,6 +3251,9 @@
   </si>
   <si>
     <t>Description pour chaque choix</t>
+  </si>
+  <si>
+    <t>Informations sur le gouvernement 5</t>
   </si>
 </sst>
 </file>
@@ -3937,6 +3940,24 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3946,6 +3967,51 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3964,15 +4030,6 @@
     <xf numFmtId="0" fontId="5" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3991,61 +4048,7 @@
     <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5230,7 +5233,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C3" sqref="C3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5240,57 +5243,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="62.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="79"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="100"/>
     </row>
     <row r="2" spans="1:13" ht="42.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="101" t="s">
         <v>397</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="82"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="103"/>
     </row>
     <row r="3" spans="1:13" ht="42.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="104" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="87" t="s">
+      <c r="B3" s="104"/>
+      <c r="C3" s="105" t="s">
         <v>398</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="105"/>
     </row>
     <row r="4" spans="1:13" ht="34.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="83" t="s">
@@ -5310,118 +5313,118 @@
       <c r="M4" s="85"/>
     </row>
     <row r="5" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="106" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="74" t="s">
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="76"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="82"/>
     </row>
     <row r="6" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="92" t="s">
+      <c r="A6" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="94"/>
-      <c r="G6" s="74" t="s">
+      <c r="B6" s="90"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="76"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="82"/>
     </row>
     <row r="7" spans="1:13" ht="19.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="95" t="s">
+      <c r="A7" s="110" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="95"/>
-      <c r="C7" s="95"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="74" t="s">
+      <c r="B7" s="110"/>
+      <c r="C7" s="110"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="75"/>
-      <c r="M7" s="76"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="82"/>
     </row>
     <row r="8" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="91" t="s">
+      <c r="A8" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="91"/>
-      <c r="E8" s="91"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="74" t="s">
+      <c r="B8" s="109"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="76"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="82"/>
     </row>
     <row r="9" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="90" t="s">
+      <c r="A9" s="108" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="74" t="s">
+      <c r="B9" s="108"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="76"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="82"/>
     </row>
     <row r="10" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="96" t="s">
+      <c r="A10" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="96"/>
-      <c r="C10" s="97" t="s">
+      <c r="B10" s="74"/>
+      <c r="C10" s="75" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="98"/>
-      <c r="G10" s="98"/>
-      <c r="H10" s="98"/>
-      <c r="I10" s="98"/>
-      <c r="J10" s="98"/>
-      <c r="K10" s="98"/>
-      <c r="L10" s="98"/>
-      <c r="M10" s="98"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
     </row>
     <row r="11" spans="1:13" ht="34.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="83" t="s">
@@ -5441,122 +5444,137 @@
       <c r="M11" s="85"/>
     </row>
     <row r="12" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="108" t="s">
+      <c r="A12" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="109"/>
-      <c r="C12" s="109"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="109"/>
-      <c r="F12" s="110"/>
-      <c r="G12" s="74" t="s">
+      <c r="B12" s="96"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="97"/>
+      <c r="G12" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="H12" s="75"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="75"/>
-      <c r="L12" s="75"/>
-      <c r="M12" s="76"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="82"/>
     </row>
     <row r="13" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="92" t="s">
+      <c r="A13" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="93"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="94"/>
-      <c r="G13" s="74" t="s">
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="H13" s="75"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="75"/>
-      <c r="L13" s="75"/>
-      <c r="M13" s="76"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="105" t="s">
+      <c r="A14" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="106"/>
-      <c r="C14" s="106"/>
-      <c r="D14" s="106"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="107"/>
-      <c r="G14" s="74" t="s">
+      <c r="B14" s="93"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="93"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="H14" s="75"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="75"/>
-      <c r="K14" s="75"/>
-      <c r="L14" s="75"/>
-      <c r="M14" s="76"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="82"/>
     </row>
     <row r="15" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="102" t="s">
+      <c r="A15" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="103"/>
-      <c r="C15" s="103"/>
-      <c r="D15" s="103"/>
-      <c r="E15" s="103"/>
-      <c r="F15" s="104"/>
-      <c r="G15" s="74" t="s">
+      <c r="B15" s="87"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="75"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="75"/>
-      <c r="K15" s="75"/>
-      <c r="L15" s="75"/>
-      <c r="M15" s="76"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="81"/>
+      <c r="L15" s="81"/>
+      <c r="M15" s="82"/>
     </row>
     <row r="16" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="99" t="s">
+      <c r="A16" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="100"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="100"/>
-      <c r="E16" s="100"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="74" t="s">
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="75"/>
-      <c r="L16" s="75"/>
-      <c r="M16" s="76"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="82"/>
     </row>
     <row r="17" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="96" t="s">
+      <c r="A17" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="96"/>
-      <c r="C17" s="97" t="s">
+      <c r="B17" s="74"/>
+      <c r="C17" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="98"/>
-      <c r="E17" s="98"/>
-      <c r="F17" s="98"/>
-      <c r="G17" s="98"/>
-      <c r="H17" s="98"/>
-      <c r="I17" s="98"/>
-      <c r="J17" s="98"/>
-      <c r="K17" s="98"/>
-      <c r="L17" s="98"/>
-      <c r="M17" s="98"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="76"/>
+      <c r="J17" s="76"/>
+      <c r="K17" s="76"/>
+      <c r="L17" s="76"/>
+      <c r="M17" s="76"/>
     </row>
     <row r="18" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="G8:M8"/>
+    <mergeCell ref="G9:M9"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="G7:M7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C17:M17"/>
     <mergeCell ref="A16:F16"/>
@@ -5572,21 +5590,6 @@
     <mergeCell ref="G14:M14"/>
     <mergeCell ref="A12:F12"/>
     <mergeCell ref="G12:M12"/>
-    <mergeCell ref="G8:M8"/>
-    <mergeCell ref="G9:M9"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:M3"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="G6:M6"/>
-    <mergeCell ref="G7:M7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5853,7 +5856,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6214,9 +6217,8 @@
       <c r="O8" s="37" t="s">
         <v>254</v>
       </c>
-      <c r="P8" s="7" t="str">
-        <f>_xlfn.TRANSLATE(Tableau1[[#This Row],[description]],"en","fr")</f>
-        <v>Informations sur la gouvernance 5</v>
+      <c r="P8" s="7" t="s">
+        <v>415</v>
       </c>
       <c r="Q8" s="37"/>
       <c r="R8" s="37"/>

</xml_diff>